<commit_message>
Started working on gas only no supplier case
</commit_message>
<xml_diff>
--- a/8.17.20 E.xlsx
+++ b/8.17.20 E.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Electric Choice Id</t>
+          <t>Electric Choice ID</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Rate Code</t>
+          <t>Electric Rate Code</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -486,7 +486,22 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Usage</t>
+          <t>Electric Usage (kWh)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Choice ID</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Rate Code</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Usage (therms)</t>
         </is>
       </c>
     </row>
@@ -539,10 +554,29 @@
           <t>Schedule GL</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>646242</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Started working on gas only no supplier case"
This reverts commit 2ed6bcc1abca584bd4b4e2f3153f327473538db8.
</commit_message>
<xml_diff>
--- a/8.17.20 E.xlsx
+++ b/8.17.20 E.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Electric Choice ID</t>
+          <t>Electric Choice Id</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Electric Rate Code</t>
+          <t>Rate Code</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -486,22 +486,7 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Electric Usage (kWh)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Gas Choice ID</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Gas Rate Code</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Gas Usage (therms)</t>
+          <t>Usage</t>
         </is>
       </c>
     </row>
@@ -554,29 +539,10 @@
           <t>Schedule GL</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>646242</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Started working on gas only no supplier case""
This reverts commit c613212fea788e8ee7bee90f690c1062651496b3.
</commit_message>
<xml_diff>
--- a/8.17.20 E.xlsx
+++ b/8.17.20 E.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Electric Choice Id</t>
+          <t>Electric Choice ID</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Rate Code</t>
+          <t>Electric Rate Code</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -486,7 +486,22 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Usage</t>
+          <t>Electric Usage (kWh)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Choice ID</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Rate Code</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Usage (therms)</t>
         </is>
       </c>
     </row>
@@ -539,10 +554,29 @@
           <t>Schedule GL</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>646242</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>